<commit_message>
modified:   api-backend/controllers/name.js 	modified:   documentation/softeng23-26-presentation_v2.xlsx
</commit_message>
<xml_diff>
--- a/documentation/softeng23-26-presentation_v2.xlsx
+++ b/documentation/softeng23-26-presentation_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voudo\Documents\codes\tl ntuaflix\NTUAflix\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voudo\Documents\codes\tl ntuaflix\NTUAflix\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1614893F-1578-4B85-B841-3DEC44190944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858295F7-2F7C-4FE8-897C-A1E525C5EE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{998E27AF-4EE8-5F42-9173-21B426B5D45A}"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="160">
   <si>
     <t>ER/JSON</t>
   </si>
@@ -445,15 +445,6 @@
     <t>dhsufcnq</t>
   </si>
   <si>
-    <t>Αναζήτηση ταινιών και σειρών με βάση το genre</t>
-  </si>
-  <si>
-    <t>Αναζήτηση ταινιών και σειρών με βάση το rating</t>
-  </si>
-  <si>
-    <t>Αναζήτηση ατόμων από τις ταινίες και σειρές με βάση το όνομα</t>
-  </si>
-  <si>
     <t>Χριστοδουλάκης</t>
   </si>
   <si>
@@ -503,6 +494,39 @@
   </si>
   <si>
     <t>03120227</t>
+  </si>
+  <si>
+    <t>Αναζήτηση ταινιών και σειρών με βάση το genre (search by genre)</t>
+  </si>
+  <si>
+    <t>Αναζήτηση ταινιών και σειρών με βάση το rating (search by rating)</t>
+  </si>
+  <si>
+    <t>Αναζήτηση ατόμων από τις ταινίες και σειρές με βάση το όνομα (search people)</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>Node.js</t>
+  </si>
+  <si>
+    <t>yaml file</t>
+  </si>
+  <si>
+    <t>Next.js/React</t>
+  </si>
+  <si>
+    <t>Node.js/Postman Scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Node.js/jest </t>
+  </si>
+  <si>
+    <t>vs code</t>
+  </si>
+  <si>
+    <t>from github</t>
   </si>
 </sst>
 </file>
@@ -768,6 +792,25 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -783,25 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1121,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A22FCA-6CEB-864C-9E7D-F12113288542}">
   <dimension ref="B1:AK50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="97" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1274,16 +1298,16 @@
     </row>
     <row r="5" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="30"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="22" t="str">
         <f>B5</f>
         <v>03120061</v>
@@ -1292,16 +1316,16 @@
     </row>
     <row r="6" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E6" s="14"/>
-      <c r="F6" s="30"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="22" t="str">
         <f t="shared" ref="G6:G10" si="0">B6</f>
         <v>03120189</v>
@@ -1310,16 +1334,16 @@
     </row>
     <row r="7" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E7" s="14"/>
-      <c r="F7" s="30"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="22" t="str">
         <f t="shared" si="0"/>
         <v>03120098</v>
@@ -1328,16 +1352,16 @@
     </row>
     <row r="8" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="22" t="str">
         <f t="shared" si="0"/>
         <v>03120227</v>
@@ -1346,16 +1370,16 @@
     </row>
     <row r="9" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E9" s="14"/>
-      <c r="F9" s="30"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="22" t="str">
         <f t="shared" si="0"/>
         <v>03120123</v>
@@ -1367,13 +1391,13 @@
         <v>128</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E10" s="14"/>
-      <c r="F10" s="30"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="22" t="str">
         <f t="shared" si="0"/>
         <v>03120890</v>
@@ -1383,18 +1407,18 @@
     <row r="11" spans="2:37" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="F11" s="30"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="2:37" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
       <c r="AK12" s="25" t="s">
         <v>121</v>
       </c>
@@ -1403,12 +1427,12 @@
       <c r="B13" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
       <c r="AK13" s="25" t="s">
         <v>122</v>
       </c>
@@ -1417,12 +1441,12 @@
       <c r="B14" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
       <c r="AK14" s="25" t="s">
         <v>127</v>
       </c>
@@ -1437,11 +1461,11 @@
       <c r="B16" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
+      <c r="C16" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="21"/>
       <c r="AK16" s="25" t="s">
         <v>123</v>
@@ -1451,11 +1475,11 @@
       <c r="B17" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
+      <c r="C17" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="21"/>
       <c r="AK17" s="25" t="s">
         <v>124</v>
@@ -1465,11 +1489,11 @@
       <c r="B18" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+      <c r="C18" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="21"/>
       <c r="AK18" s="25" t="s">
         <v>125</v>
@@ -1483,96 +1507,114 @@
       <c r="C20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="32"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="21" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
     </row>
     <row r="22" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
+      <c r="C23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
+      <c r="C26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="C27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="C28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
     </row>
     <row r="30" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
+      <c r="C30" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
@@ -1580,17 +1622,21 @@
       <c r="B32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="C32" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
+      <c r="C33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
@@ -1628,9 +1674,11 @@
       <c r="B34" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
+      <c r="C34" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
       <c r="H34" s="20"/>
@@ -1668,9 +1716,11 @@
       <c r="B35" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
+      <c r="C35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="20"/>
@@ -1705,60 +1755,70 @@
       <c r="AK35" s="4"/>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
     </row>
     <row r="37" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
+      <c r="C37" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
+      <c r="C38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
+      <c r="C39" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
     </row>
     <row r="41" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
+      <c r="C41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" spans="2:37" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
+      <c r="C42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
       <c r="H42" s="20"/>
@@ -1796,9 +1856,11 @@
       <c r="B43" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
+      <c r="C43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="23"/>
       <c r="G43" s="23"/>
       <c r="H43" s="20"/>
@@ -1838,38 +1900,53 @@
       </c>
     </row>
     <row r="46" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
     </row>
     <row r="47" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
     </row>
     <row r="48" spans="2:37" x14ac:dyDescent="0.3">
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0"/>
   <mergeCells count="31">
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F5:F14"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B46:E50"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="D37:E37"/>
@@ -1886,21 +1963,6 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B46:E50"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F5:F14"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>